<commit_message>
990423 W naghdinegi added.
</commit_message>
<xml_diff>
--- a/Main/طلا و سکه.xlsx
+++ b/Main/طلا و سکه.xlsx
@@ -680,73 +680,34 @@
     <xf numFmtId="164" fontId="2" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,6 +718,45 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,7 +1250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1277,33 +1279,33 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="71">
-        <v>19595</v>
-      </c>
-      <c r="D2" s="72"/>
+      <c r="C2" s="56">
+        <v>21850</v>
+      </c>
+      <c r="D2" s="57"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="57" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="65" t="s">
+      <c r="I2" s="69"/>
+      <c r="J2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="66"/>
+      <c r="K2" s="51"/>
     </row>
     <row r="3" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="53">
-        <v>20250</v>
-      </c>
-      <c r="D3" s="54"/>
+      <c r="C3" s="58">
+        <v>22000</v>
+      </c>
+      <c r="D3" s="59"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="42" t="s">
         <v>20</v>
       </c>
@@ -1321,12 +1323,12 @@
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="53">
-        <v>5564</v>
-      </c>
-      <c r="D4" s="54"/>
+      <c r="C4" s="58">
+        <v>6041</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="60" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1334,12 +1336,12 @@
       </c>
       <c r="H4" s="7">
         <f>0.23533*C2*C5+30000</f>
-        <v>8215042.1462500012</v>
+        <v>9162121.8480000012</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="22">
         <f>C5/41.41333*C2</f>
-        <v>839853.37571260263</v>
+        <v>937031.62725624815</v>
       </c>
       <c r="K4" s="27"/>
       <c r="M4" s="1"/>
@@ -1348,52 +1350,52 @@
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="53">
-        <v>1775</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="58">
+        <v>1776</v>
+      </c>
+      <c r="D5" s="59"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="74"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="28">
         <f>C7-H4</f>
-        <v>254957.85374999885</v>
+        <v>1040878.1519999988</v>
       </c>
       <c r="I5" s="29">
         <f>H5/H4</f>
-        <v>3.1035489436457959E-2</v>
+        <v>0.11360666985969108</v>
       </c>
       <c r="J5" s="30">
         <f>C6-J4</f>
-        <v>-4853.3757126026321</v>
+        <v>1968.3727437518537</v>
       </c>
       <c r="K5" s="31">
         <f>J5/J4</f>
-        <v>-5.7788369410132065E-3</v>
+        <v>2.1006470715567074E-3</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="53">
-        <v>835000</v>
-      </c>
-      <c r="D6" s="54"/>
+      <c r="C6" s="58">
+        <v>939000</v>
+      </c>
+      <c r="D6" s="59"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="75"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="32">
         <f>C8-H4</f>
-        <v>334957.85374999885</v>
+        <v>957878.15199999884</v>
       </c>
       <c r="I6" s="33">
         <f>H6/H4</f>
-        <v>4.0773723102918012E-2</v>
+        <v>0.10454763294913984</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="34"/>
@@ -1402,12 +1404,12 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="53">
-        <v>8470000</v>
-      </c>
-      <c r="D7" s="54"/>
+      <c r="C7" s="58">
+        <v>10203000</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="70" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="12" t="s">
@@ -1415,12 +1417,12 @@
       </c>
       <c r="H7" s="8">
         <f>0.23533*C3*C5+30000</f>
-        <v>8488642.6875</v>
+        <v>9224813.7599999998</v>
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="24">
         <f>C5/41.41333*C3</f>
-        <v>867927.0659954173</v>
+        <v>943464.33865617658</v>
       </c>
       <c r="K7" s="35"/>
     </row>
@@ -1428,51 +1430,51 @@
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="53">
-        <v>8550000</v>
-      </c>
-      <c r="D8" s="54"/>
+      <c r="C8" s="58">
+        <v>10120000</v>
+      </c>
+      <c r="D8" s="59"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="60"/>
+      <c r="F8" s="71"/>
       <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="28">
         <f>C7-H7</f>
-        <v>-18642.6875</v>
+        <v>978186.24000000022</v>
       </c>
       <c r="I8" s="29">
         <f>H8/H7</f>
-        <v>-2.1961918043095861E-3</v>
+        <v>0.10603858955305351</v>
       </c>
       <c r="J8" s="30">
         <f>C6-J7</f>
-        <v>-32927.065995417302</v>
+        <v>-4464.3386561765801</v>
       </c>
       <c r="K8" s="31">
         <f>J8/J7</f>
-        <v>-3.7937595548600114E-2</v>
+        <v>-4.7318573402947706E-3</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="53">
-        <v>4400000</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="F9" s="61"/>
+      <c r="C9" s="58">
+        <v>5200000</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="32">
         <f>C8-H7</f>
-        <v>61357.3125</v>
+        <v>895186.24000000022</v>
       </c>
       <c r="I9" s="33">
         <f>H9/H7</f>
-        <v>7.2281652978929203E-3</v>
+        <v>9.7041117933637316E-2</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="34"/>
@@ -1481,11 +1483,11 @@
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="55">
-        <v>2450000</v>
-      </c>
-      <c r="D10" s="56"/>
-      <c r="F10" s="62" t="s">
+      <c r="C10" s="66">
+        <v>2950000</v>
+      </c>
+      <c r="D10" s="67"/>
+      <c r="F10" s="73" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="15" t="s">
@@ -1493,35 +1495,35 @@
       </c>
       <c r="H10" s="8">
         <f>0.23533*C12*C5 + 30000</f>
-        <v>8580753.0874882992</v>
+        <v>9319036.819908049</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="24">
         <f>C12*C5/41.41333</f>
-        <v>877378.35885208927</v>
+        <v>953132.40798554476</v>
       </c>
       <c r="K10" s="35"/>
     </row>
     <row r="11" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="63"/>
+      <c r="F11" s="74"/>
       <c r="G11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="28">
         <f>C7-H10</f>
-        <v>-110753.08748829924</v>
+        <v>883963.18009195104</v>
       </c>
       <c r="I11" s="29">
         <f>H11/H10</f>
-        <v>-1.2907152362860745E-2</v>
+        <v>9.4855637677443275E-2</v>
       </c>
       <c r="J11" s="30">
         <f>C6-J10</f>
-        <v>-42378.358852089266</v>
+        <v>-14132.407985544764</v>
       </c>
       <c r="K11" s="31">
         <f>J11/J10</f>
-        <v>-4.8301121659228799E-2</v>
+        <v>-1.4827329201211145E-2</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1530,23 +1532,23 @@
       </c>
       <c r="C12" s="3">
         <f>3.6791*C4</f>
-        <v>20470.5124</v>
+        <v>22225.4431</v>
       </c>
       <c r="D12" s="40">
         <f>(C12-C3)/C12</f>
-        <v>1.0772197377921991E-2</v>
-      </c>
-      <c r="F12" s="64"/>
+        <v>1.0143469310629871E-2</v>
+      </c>
+      <c r="F12" s="75"/>
       <c r="G12" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="32">
         <f>C8-H10</f>
-        <v>-30753.087488299236</v>
+        <v>800963.18009195104</v>
       </c>
       <c r="I12" s="33">
         <f>H12/H10</f>
-        <v>-3.5839613580235384E-3</v>
+        <v>8.5949137831591291E-2</v>
       </c>
       <c r="J12" s="23"/>
       <c r="K12" s="34"/>
@@ -1557,13 +1559,13 @@
       </c>
       <c r="C13" s="21">
         <f>C3-C2</f>
-        <v>655</v>
+        <v>150</v>
       </c>
       <c r="D13" s="41">
         <f>C13/C3</f>
-        <v>3.2345679012345682E-2</v>
-      </c>
-      <c r="F13" s="50" t="s">
+        <v>6.8181818181818179E-3</v>
+      </c>
+      <c r="F13" s="63" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="18" t="s">
@@ -1571,7 +1573,7 @@
       </c>
       <c r="H13" s="7">
         <f>8.13*21.6/18*C6+30000</f>
-        <v>8176260.0000000019</v>
+        <v>9190884.0000000019</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="36"/>
@@ -1583,23 +1585,23 @@
       </c>
       <c r="C14" s="21">
         <f>C8-C7</f>
-        <v>80000</v>
+        <v>-83000</v>
       </c>
       <c r="D14" s="41">
         <f>C14/C8</f>
-        <v>9.3567251461988306E-3</v>
-      </c>
-      <c r="F14" s="51"/>
+        <v>-8.2015810276679837E-3</v>
+      </c>
+      <c r="F14" s="64"/>
       <c r="G14" s="19" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="28">
         <f>C7-H13</f>
-        <v>293739.99999999814</v>
+        <v>1012115.9999999981</v>
       </c>
       <c r="I14" s="29">
         <f>H14/H13</f>
-        <v>3.592596125857031E-2</v>
+        <v>0.11012172496138542</v>
       </c>
       <c r="J14" s="37"/>
       <c r="K14" s="38"/>
@@ -1610,23 +1612,23 @@
       </c>
       <c r="C15" s="21">
         <f>C9 - C7/2 + 30000</f>
-        <v>195000</v>
+        <v>128500</v>
       </c>
       <c r="D15" s="41">
         <f>C15/C9</f>
-        <v>4.4318181818181819E-2</v>
-      </c>
-      <c r="F15" s="52"/>
+        <v>2.4711538461538462E-2</v>
+      </c>
+      <c r="F15" s="65"/>
       <c r="G15" s="20" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="32">
         <f>C8-H13</f>
-        <v>373739.99999999814</v>
+        <v>929115.99999999814</v>
       </c>
       <c r="I15" s="33">
         <f>H15/H13</f>
-        <v>4.5710385922169555E-2</v>
+        <v>0.10109103759768896</v>
       </c>
       <c r="J15" s="39"/>
       <c r="K15" s="34"/>
@@ -1637,11 +1639,11 @@
       </c>
       <c r="C16" s="21">
         <f>C10-C7/4 + 30000</f>
-        <v>362500</v>
+        <v>429250</v>
       </c>
       <c r="D16" s="41">
         <f>C16/C10</f>
-        <v>0.14795918367346939</v>
+        <v>0.1455084745762712</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1650,11 +1652,11 @@
       </c>
       <c r="C17" s="48">
         <f>2200*(C3-C2)</f>
-        <v>1441000</v>
+        <v>330000</v>
       </c>
       <c r="D17" s="49">
         <f>C17/(2200*C2)</f>
-        <v>3.3426894615973465E-2</v>
+        <v>6.8649885583524023E-3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
@@ -1662,12 +1664,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:F6"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
@@ -1678,6 +1674,12 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F10:F12"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:I6 H8:I9 H11:I12 H14:I15">
     <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">

</xml_diff>

<commit_message>
Risk management has been added.
</commit_message>
<xml_diff>
--- a/Main/طلا و سکه.xlsx
+++ b/Main/طلا و سکه.xlsx
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,14 +110,6 @@
       <charset val="178"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="B Nazanin"/>
-      <charset val="178"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="B Nazanin"/>
       <charset val="178"/>
@@ -533,157 +525,157 @@
   </cellStyleXfs>
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="13" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,64 +690,64 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1250,40 +1242,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" style="2"/>
-    <col min="15" max="15" width="8.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="8.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="56">
-        <v>20343</v>
+        <v>20842</v>
       </c>
       <c r="D2" s="57"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="52"/>
       <c r="G2" s="53"/>
       <c r="H2" s="68" t="s">
@@ -1295,372 +1287,372 @@
       </c>
       <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="58">
-        <v>21650</v>
+        <v>21500</v>
       </c>
       <c r="D3" s="59"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="54"/>
       <c r="G3" s="55"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="58">
-        <v>6043</v>
+        <v>5863</v>
       </c>
       <c r="D4" s="59"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="60" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="10">
         <f>0.23533*C2*C5+30000</f>
-        <v>8929624.5152100008</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="22">
+        <v>8735927.4515000004</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12">
         <f>C5/41.41333*C2</f>
-        <v>913175.46789886255</v>
-      </c>
-      <c r="K4" s="27"/>
-      <c r="M4" s="1"/>
+        <v>893300.53873957961</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="58">
-        <v>1859</v>
+        <v>1775</v>
       </c>
       <c r="D5" s="59"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="61"/>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="15">
         <f>C7-H4</f>
-        <v>1170375.4847899992</v>
-      </c>
-      <c r="I5" s="29">
+        <v>543072.54849999957</v>
+      </c>
+      <c r="I5" s="16">
         <f>H5/H4</f>
-        <v>0.13106659555465924</v>
-      </c>
-      <c r="J5" s="30">
+        <v>6.216541420645056E-2</v>
+      </c>
+      <c r="J5" s="17">
         <f>C6-J4</f>
-        <v>53224.532101137447</v>
-      </c>
-      <c r="K5" s="31">
+        <v>16299.461260420387</v>
+      </c>
+      <c r="K5" s="18">
         <f>J5/J4</f>
-        <v>5.8285109458319627E-2</v>
+        <v>1.824633541967683E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="58">
-        <v>966400</v>
+        <v>909600</v>
       </c>
       <c r="D6" s="59"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="62"/>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="20">
         <f>C8-H4</f>
-        <v>1390375.4847899992</v>
-      </c>
-      <c r="I6" s="33">
+        <v>363072.54849999957</v>
+      </c>
+      <c r="I6" s="21">
         <f>H6/H4</f>
-        <v>0.15570368971525578</v>
-      </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="34"/>
+        <v>4.1560847490515536E-2</v>
+      </c>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="58">
-        <v>10100000</v>
+        <v>9279000</v>
       </c>
       <c r="D7" s="59"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="25">
         <f>0.23533*C3*C5+30000</f>
-        <v>9501408.875500001</v>
+        <v>9010781.125</v>
       </c>
       <c r="I7" s="26"/>
-      <c r="J7" s="24">
+      <c r="J7" s="27">
         <f>C5/41.41333*C3</f>
-        <v>971845.29715432203</v>
-      </c>
-      <c r="K7" s="35"/>
+        <v>921502.8108099493</v>
+      </c>
+      <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="58">
-        <v>10320000</v>
+        <v>9099000</v>
       </c>
       <c r="D8" s="59"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="71"/>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="15">
         <f>C7-H7</f>
-        <v>598591.12449999899</v>
-      </c>
-      <c r="I8" s="29">
+        <v>268218.875</v>
+      </c>
+      <c r="I8" s="16">
         <f>H8/H7</f>
-        <v>6.3000248946606746E-2</v>
-      </c>
-      <c r="J8" s="30">
+        <v>2.9766439921156115E-2</v>
+      </c>
+      <c r="J8" s="17">
         <f>C6-J7</f>
-        <v>-5445.2971543220337</v>
-      </c>
-      <c r="K8" s="31">
+        <v>-11902.810809949297</v>
+      </c>
+      <c r="K8" s="18">
         <f>J8/J7</f>
-        <v>-5.6030493436213646E-3</v>
+        <v>-1.2916738473632427E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="58">
-        <v>5150000</v>
+        <v>5100000</v>
       </c>
       <c r="D9" s="59"/>
       <c r="F9" s="72"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="20">
         <f>C8-H7</f>
-        <v>818591.12449999899</v>
-      </c>
-      <c r="I9" s="33">
+        <v>88218.875</v>
+      </c>
+      <c r="I9" s="21">
         <f>H9/H7</f>
-        <v>8.6154709814750666E-2</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="34"/>
+        <v>9.7903693116283518E-3</v>
+      </c>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
     </row>
-    <row r="10" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="66">
-        <v>3140000</v>
+        <v>3200000</v>
       </c>
       <c r="D10" s="67"/>
       <c r="F10" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="25">
         <f>0.23533*C12*C5 + 30000</f>
-        <v>9756371.8965380099</v>
+        <v>9040256.1739654765</v>
       </c>
       <c r="I10" s="26"/>
-      <c r="J10" s="24">
+      <c r="J10" s="27">
         <f>C12*C5/41.41333</f>
-        <v>998006.62290861423</v>
-      </c>
-      <c r="K10" s="35"/>
+        <v>924527.1958932064</v>
+      </c>
+      <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F11" s="74"/>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="15">
         <f>C7-H10</f>
-        <v>343628.10346199013</v>
-      </c>
-      <c r="I11" s="29">
+        <v>238743.82603452355</v>
+      </c>
+      <c r="I11" s="16">
         <f>H11/H10</f>
-        <v>3.5220890214724646E-2</v>
-      </c>
-      <c r="J11" s="30">
+        <v>2.6408966896543089E-2</v>
+      </c>
+      <c r="J11" s="17">
         <f>C6-J10</f>
-        <v>-31606.622908614227</v>
-      </c>
-      <c r="K11" s="31">
+        <v>-14927.195893206401</v>
+      </c>
+      <c r="K11" s="18">
         <f>J11/J10</f>
-        <v>-3.1669752668072614E-2</v>
+        <v>-1.6145761811565643E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="34">
         <f>3.6791*C4</f>
-        <v>22232.801299999999</v>
-      </c>
-      <c r="D12" s="40">
+        <v>21570.563300000002</v>
+      </c>
+      <c r="D12" s="35">
         <f>(C12-C3)/C12</f>
-        <v>2.6213579302757462E-2</v>
+        <v>3.2712775748420819E-3</v>
       </c>
       <c r="F12" s="75"/>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="20">
         <f>C8-H10</f>
-        <v>563628.10346199013</v>
-      </c>
-      <c r="I12" s="33">
+        <v>58743.826034523547</v>
+      </c>
+      <c r="I12" s="21">
         <f>H12/H10</f>
-        <v>5.7770256140193897E-2</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="34"/>
+        <v>6.4980267045635911E-3</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="37">
         <f>C3-C2</f>
-        <v>1307</v>
-      </c>
-      <c r="D13" s="41">
+        <v>658</v>
+      </c>
+      <c r="D13" s="38">
         <f>C13/C3</f>
-        <v>6.0369515011547345E-2</v>
+        <v>3.0604651162790698E-2</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="10">
         <f>8.13*21.6/18*C6+30000</f>
-        <v>9458198.4000000022</v>
-      </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="27"/>
+        <v>8904057.6000000015</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="37">
         <f>C8-C7</f>
-        <v>220000</v>
-      </c>
-      <c r="D14" s="41">
+        <v>-180000</v>
+      </c>
+      <c r="D14" s="38">
         <f>C14/C8</f>
-        <v>2.1317829457364341E-2</v>
+        <v>-1.9782393669634024E-2</v>
       </c>
       <c r="F14" s="64"/>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="15">
         <f>C7-H13</f>
-        <v>641801.59999999776</v>
-      </c>
-      <c r="I14" s="29">
+        <v>374942.39999999851</v>
+      </c>
+      <c r="I14" s="16">
         <f>H14/H13</f>
-        <v>6.7856643819186283E-2</v>
-      </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
+        <v>4.2109161557984359E-2</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
     </row>
-    <row r="15" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="37">
         <f>C9 - C7/2 + 30000</f>
-        <v>130000</v>
-      </c>
-      <c r="D15" s="41">
+        <v>490500</v>
+      </c>
+      <c r="D15" s="38">
         <f>C15/C9</f>
-        <v>2.524271844660194E-2</v>
+        <v>9.6176470588235294E-2</v>
       </c>
       <c r="F15" s="65"/>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="20">
         <f>C8-H13</f>
-        <v>861801.59999999776</v>
-      </c>
-      <c r="I15" s="33">
+        <v>194942.39999999851</v>
+      </c>
+      <c r="I15" s="21">
         <f>H15/H13</f>
-        <v>9.1116887545940842E-2</v>
-      </c>
-      <c r="J15" s="39"/>
-      <c r="K15" s="34"/>
+        <v>2.1893658908944891E-2</v>
+      </c>
+      <c r="J15" s="45"/>
+      <c r="K15" s="23"/>
     </row>
-    <row r="16" spans="2:13" ht="19.5" x14ac:dyDescent="0.5">
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="37">
         <f>C10-C7/4 + 30000</f>
-        <v>645000</v>
-      </c>
-      <c r="D16" s="41">
+        <v>910250</v>
+      </c>
+      <c r="D16" s="38">
         <f>C16/C10</f>
-        <v>0.20541401273885351</v>
+        <v>0.28445312499999997</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="47" t="s">
+    <row r="17" spans="2:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="47">
         <f>2200*(C3-C2)</f>
-        <v>2875400</v>
-      </c>
-      <c r="D17" s="49">
+        <v>1447600</v>
+      </c>
+      <c r="D17" s="48">
         <f>C17/(2200*C2)</f>
-        <v>6.4248144324829184E-2</v>
+        <v>3.1570866519527875E-2</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="46"/>
+      <c r="B18" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1760,6 +1752,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>